<commit_message>
Changed column names to remove spaces
</commit_message>
<xml_diff>
--- a/PepsiChallenge/Pepsi Challenge Results.xlsx
+++ b/PepsiChallenge/Pepsi Challenge Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\Documents\Work\Blog\Data_Team_Blog_Posts\PepsiChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,21 +32,12 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Pre-Tell</t>
-  </si>
-  <si>
-    <t>Gen Pref</t>
-  </si>
-  <si>
     <t>Which</t>
   </si>
   <si>
     <t>Conf</t>
   </si>
   <si>
-    <t>Act Pref</t>
-  </si>
-  <si>
     <t>Gillian</t>
   </si>
   <si>
@@ -138,6 +129,15 @@
   </si>
   <si>
     <t>Steph</t>
+  </si>
+  <si>
+    <t>Pre_Tell</t>
+  </si>
+  <si>
+    <t>Gen_Pref</t>
+  </si>
+  <si>
+    <t>Act_Pref</t>
   </si>
 </sst>
 </file>
@@ -478,568 +478,568 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>